<commit_message>
Pushing HW3 code (yeehaw)
</commit_message>
<xml_diff>
--- a/Working/HW2_BoxModel_manual/starter_code/homconmodel-modflow_as_dh.xlsx
+++ b/Working/HW2_BoxModel_manual/starter_code/homconmodel-modflow_as_dh.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnahh\Desktop\GW_Modeling\homework-hsiehdf\Working\HW2_BoxModel_manual\starter_code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24500EC5-DA7F-4C50-B421-393455828158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA1D3AE-4B75-45E3-9FF9-16E7D71A4723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30915" yWindow="4050" windowWidth="4860" windowHeight="915" xr2:uid="{288C77B4-A716-8B43-9660-12AFA9E6387F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{288C77B4-A716-8B43-9660-12AFA9E6387F}"/>
   </bookViews>
   <sheets>
     <sheet name="Homogeneous conceptual modflow" sheetId="1" r:id="rId1"/>
@@ -409,7 +409,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> (m)</a:t>
+                  <a:t> (100m)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1266,7 +1266,7 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>105410</xdr:rowOff>
+      <xdr:rowOff>103505</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1314,7 +1314,7 @@
       <xdr:col>28</xdr:col>
       <xdr:colOff>135073</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>162045</xdr:rowOff>
+      <xdr:rowOff>160140</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1739,7 +1739,7 @@
       <xdr:col>13</xdr:col>
       <xdr:colOff>228703</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>47209</xdr:rowOff>
+      <xdr:rowOff>49114</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
@@ -2123,7 +2123,7 @@
   <dimension ref="A1:AL55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="W24" sqref="W24"/>
+      <selection activeCell="AN12" sqref="AN12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>

</xml_diff>